<commit_message>
Update to UNFCCC inventory files
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/Edgar_scaling_mapping.xlsx
+++ b/input/mappings/scaling/Edgar_scaling_mapping.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10715"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emcduffie/Documents/GEOS-Chem/CEDS_Emissions/CEDS_v0611/input/mappings/scaling/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69137149-AC78-1D46-8B97-B2FF568772AE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14640" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="14640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
     <sheet name="method" sheetId="2" r:id="rId2"/>
     <sheet name="year" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="175">
   <si>
     <t>pre_ext_method</t>
   </si>
@@ -543,12 +549,15 @@
   </si>
   <si>
     <t>1A3dii_Domestic-navigation</t>
+  </si>
+  <si>
+    <t>Domestic aviation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1005,13 +1014,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="405">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1422,6 +1432,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1746,17 +1764,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="27.1640625" customWidth="1"/>
     <col min="4" max="4" width="26.5" customWidth="1"/>
@@ -1764,7 +1782,7 @@
     <col min="8" max="8" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1781,7 +1799,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1795,7 +1813,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>40</v>
       </c>
@@ -1803,7 +1821,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>40</v>
       </c>
@@ -1811,7 +1829,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -1826,7 +1844,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -1840,7 +1858,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>42</v>
       </c>
@@ -1848,7 +1866,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>42</v>
       </c>
@@ -1856,7 +1874,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>42</v>
       </c>
@@ -1864,7 +1882,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>42</v>
       </c>
@@ -1872,7 +1890,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>42</v>
       </c>
@@ -1880,7 +1898,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>42</v>
       </c>
@@ -1888,7 +1906,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>42</v>
       </c>
@@ -1896,7 +1914,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>42</v>
       </c>
@@ -1904,7 +1922,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>42</v>
       </c>
@@ -1912,7 +1930,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
         <v>42</v>
       </c>
@@ -1920,7 +1938,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
         <v>42</v>
       </c>
@@ -1928,7 +1946,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>42</v>
       </c>
@@ -1936,11 +1954,13 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="1"/>
+      <c r="B19" s="6" t="s">
+        <v>174</v>
+      </c>
       <c r="C19" s="1" t="s">
         <v>31</v>
       </c>
@@ -1948,7 +1968,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -1962,7 +1982,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -1976,7 +1996,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -1987,7 +2007,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -2001,7 +2021,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -2015,7 +2035,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
         <v>43</v>
       </c>
@@ -2023,7 +2043,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
         <v>43</v>
       </c>
@@ -2031,7 +2051,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>120</v>
       </c>
@@ -2042,7 +2062,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>72</v>
       </c>
@@ -2056,7 +2076,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -2071,7 +2091,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" t="s">
@@ -2081,7 +2101,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -2089,7 +2109,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -2097,7 +2117,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>86</v>
       </c>
@@ -2111,7 +2131,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>88</v>
       </c>
@@ -2125,7 +2145,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>90</v>
       </c>
@@ -2139,7 +2159,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>92</v>
       </c>
@@ -2153,7 +2173,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -2168,7 +2188,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>46</v>
       </c>
@@ -2182,7 +2202,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>47</v>
       </c>
@@ -2196,7 +2216,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>78</v>
       </c>
@@ -2211,7 +2231,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>79</v>
       </c>
@@ -2226,7 +2246,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>80</v>
       </c>
@@ -2241,7 +2261,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>81</v>
       </c>
@@ -2256,7 +2276,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>100</v>
       </c>
@@ -2270,7 +2290,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>93</v>
       </c>
@@ -2284,7 +2304,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>98</v>
       </c>
@@ -2298,7 +2318,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>95</v>
       </c>
@@ -2313,7 +2333,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>105</v>
       </c>
@@ -2327,7 +2347,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>107</v>
       </c>
@@ -2342,12 +2362,12 @@
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D50" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -2358,7 +2378,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -2369,7 +2389,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -2382,7 +2402,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>51</v>
       </c>
@@ -2393,7 +2413,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -2404,7 +2424,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>102</v>
       </c>
@@ -2418,7 +2438,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>74</v>
       </c>
@@ -2433,7 +2453,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>53</v>
       </c>
@@ -2447,7 +2467,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>76</v>
       </c>
@@ -2462,7 +2482,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>54</v>
       </c>
@@ -2473,53 +2493,53 @@
         <v>39</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="3"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="3"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="3"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="3"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D78" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="A1:C84">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C84">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2533,21 +2553,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2564,7 +2584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2593,20 +2613,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2632,7 +2652,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>137</v>
       </c>
@@ -2655,7 +2675,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>144</v>
       </c>
@@ -2681,7 +2701,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>136</v>
       </c>
@@ -2707,7 +2727,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>136</v>
       </c>
@@ -2733,7 +2753,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>136</v>
       </c>
@@ -2759,7 +2779,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>141</v>
       </c>
@@ -2785,7 +2805,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>148</v>
       </c>
@@ -2811,7 +2831,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>149</v>
       </c>
@@ -2837,7 +2857,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>150</v>
       </c>
@@ -2863,7 +2883,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>151</v>
       </c>
@@ -2889,7 +2909,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>152</v>
       </c>
@@ -2915,7 +2935,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>153</v>
       </c>
@@ -2941,7 +2961,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>154</v>
       </c>
@@ -2967,7 +2987,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>155</v>
       </c>
@@ -2993,7 +3013,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>156</v>
       </c>
@@ -3019,7 +3039,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>157</v>
       </c>
@@ -3045,7 +3065,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>158</v>
       </c>
@@ -3071,7 +3091,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>159</v>
       </c>
@@ -3097,7 +3117,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>160</v>
       </c>
@@ -3123,7 +3143,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>161</v>
       </c>
@@ -3149,7 +3169,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>162</v>
       </c>
@@ -3175,7 +3195,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>163</v>
       </c>
@@ -3201,7 +3221,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>164</v>
       </c>
@@ -3227,7 +3247,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>144</v>
       </c>
@@ -3253,7 +3273,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>165</v>
       </c>
@@ -3279,7 +3299,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>166</v>
       </c>
@@ -3305,7 +3325,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>167</v>
       </c>
@@ -3331,7 +3351,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -3357,7 +3377,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>168</v>
       </c>
@@ -3383,7 +3403,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>137</v>
       </c>
@@ -3409,7 +3429,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>171</v>
       </c>

</xml_diff>

<commit_message>
Changes required to update EDGAR scaling inventory Now uses EDGAR v4.3.2 for all species, including CH4.
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/Edgar_scaling_mapping.xlsx
+++ b/input/mappings/scaling/Edgar_scaling_mapping.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10812"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emcduffie/Documents/GEOS-Chem/CEDS_Emissions/CEDS_v0611/input/mappings/scaling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69137149-AC78-1D46-8B97-B2FF568772AE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06366EB6-21C9-9F42-A945-FD8F6EE79A35}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="14640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13040" yWindow="3500" windowWidth="25360" windowHeight="14640" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
     <sheet name="method" sheetId="2" r:id="rId2"/>
     <sheet name="year" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="180">
   <si>
     <t>pre_ext_method</t>
   </si>
@@ -552,6 +558,21 @@
   </si>
   <si>
     <t>Domestic aviation</t>
+  </si>
+  <si>
+    <t>Fugitive emissions from oil and gas</t>
+  </si>
+  <si>
+    <t>Production of metals</t>
+  </si>
+  <si>
+    <t>Production of pulp/paper/food/drink</t>
+  </si>
+  <si>
+    <t>Agricultural waste burning</t>
+  </si>
+  <si>
+    <t>Fossil fuel fires</t>
   </si>
 </sst>
 </file>
@@ -1767,11 +1788,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomRight" activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2080,8 +2101,8 @@
       <c r="A29" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>119</v>
+      <c r="B29" s="6" t="s">
+        <v>175</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" t="s">
@@ -2192,8 +2213,8 @@
       <c r="A38" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>123</v>
+      <c r="B38" s="6" t="s">
+        <v>176</v>
       </c>
       <c r="D38" t="s">
         <v>29</v>
@@ -2206,8 +2227,8 @@
       <c r="A39" t="s">
         <v>47</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>104</v>
+      <c r="B39" s="6" t="s">
+        <v>177</v>
       </c>
       <c r="D39" t="s">
         <v>63</v>
@@ -2381,6 +2402,9 @@
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>49</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>178</v>
       </c>
       <c r="D52" t="s">
         <v>64</v>
@@ -2485,6 +2509,9 @@
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>54</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>179</v>
       </c>
       <c r="C60" t="s">
         <v>54</v>
@@ -2616,9 +2643,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2672,7 +2699,7 @@
         <v>1992</v>
       </c>
       <c r="G2">
-        <v>2009</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -2695,7 +2722,7 @@
         <v>2000</v>
       </c>
       <c r="G3">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="H3" t="s">
         <v>145</v>
@@ -2825,7 +2852,7 @@
         <v>1992</v>
       </c>
       <c r="G8">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="H8" t="s">
         <v>147</v>
@@ -2851,7 +2878,7 @@
         <v>1992</v>
       </c>
       <c r="G9">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="H9" t="s">
         <v>147</v>
@@ -2877,7 +2904,7 @@
         <v>1992</v>
       </c>
       <c r="G10">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="H10" t="s">
         <v>147</v>
@@ -2903,7 +2930,7 @@
         <v>1992</v>
       </c>
       <c r="G11">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="H11" t="s">
         <v>147</v>
@@ -2929,7 +2956,7 @@
         <v>1992</v>
       </c>
       <c r="G12">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="H12" t="s">
         <v>147</v>
@@ -2955,7 +2982,7 @@
         <v>1992</v>
       </c>
       <c r="G13">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="H13" t="s">
         <v>147</v>
@@ -2981,7 +3008,7 @@
         <v>1992</v>
       </c>
       <c r="G14">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="H14" t="s">
         <v>147</v>
@@ -3007,7 +3034,7 @@
         <v>1992</v>
       </c>
       <c r="G15">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="H15" t="s">
         <v>147</v>
@@ -3033,7 +3060,7 @@
         <v>1992</v>
       </c>
       <c r="G16">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="H16" t="s">
         <v>147</v>
@@ -3059,7 +3086,7 @@
         <v>1992</v>
       </c>
       <c r="G17">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="H17" t="s">
         <v>147</v>
@@ -3085,7 +3112,7 @@
         <v>1992</v>
       </c>
       <c r="G18">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="H18" t="s">
         <v>147</v>
@@ -3111,7 +3138,7 @@
         <v>1992</v>
       </c>
       <c r="G19">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="H19" t="s">
         <v>147</v>
@@ -3137,7 +3164,7 @@
         <v>1992</v>
       </c>
       <c r="G20">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="H20" t="s">
         <v>147</v>
@@ -3163,7 +3190,7 @@
         <v>1992</v>
       </c>
       <c r="G21">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="H21" t="s">
         <v>147</v>
@@ -3189,7 +3216,7 @@
         <v>1992</v>
       </c>
       <c r="G22">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="H22" t="s">
         <v>147</v>
@@ -3215,7 +3242,7 @@
         <v>1992</v>
       </c>
       <c r="G23">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="H23" t="s">
         <v>169</v>
@@ -3241,7 +3268,7 @@
         <v>1992</v>
       </c>
       <c r="G24">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="H24" t="s">
         <v>169</v>
@@ -3267,7 +3294,7 @@
         <v>1992</v>
       </c>
       <c r="G25">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="H25" t="s">
         <v>169</v>
@@ -3293,7 +3320,7 @@
         <v>1992</v>
       </c>
       <c r="G26">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="H26" t="s">
         <v>169</v>
@@ -3319,7 +3346,7 @@
         <v>1992</v>
       </c>
       <c r="G27">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="H27" t="s">
         <v>169</v>
@@ -3345,7 +3372,7 @@
         <v>1992</v>
       </c>
       <c r="G28">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="H28" t="s">
         <v>169</v>
@@ -3371,7 +3398,7 @@
         <v>1992</v>
       </c>
       <c r="G29">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="H29" t="s">
         <v>169</v>
@@ -3397,7 +3424,7 @@
         <v>1992</v>
       </c>
       <c r="G30">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="H30" t="s">
         <v>169</v>
@@ -3423,7 +3450,7 @@
         <v>2000</v>
       </c>
       <c r="G31">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>170</v>

</xml_diff>

<commit_message>
Debugging Updates to scaling inventories 1 - Don't try to load inventory data for species that don't exist (i.e., BC & OC) 2 - Only scale 1A3e to Edgar from 1920-2011 (not 2012). Scaling factor for 2012 is 24 and results in too large Irn emissions as 1A3e emissions significantly increase after 2013 and a scaling factor of 24 from 2012 is not valid. 3 - scale tur, mlt, and bhr to Edgar v4.3.2. Were origianlly scaled to Edgar v4.2 and not 4.3.1 Since I am not longer scaling to Edgar v4.2, need to scale these to Edgar v4.3.2. Results in too low emissions for Turkey (relative to GAINS) otherwise.
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/Edgar_scaling_mapping.xlsx
+++ b/input/mappings/scaling/Edgar_scaling_mapping.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emcduffie/Documents/GEOS-Chem/CEDS_Emissions/CEDS_v0611/input/mappings/scaling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emcduffie/Documents/GEOS-Chem/CEDS/CEDS_v0611/input/mappings/scaling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06366EB6-21C9-9F42-A945-FD8F6EE79A35}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A46E3C-CB9B-D84C-82CD-A97A20FF4FE2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13040" yWindow="3500" windowWidth="25360" windowHeight="14640" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13040" yWindow="3420" windowWidth="25360" windowHeight="14640" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="182">
   <si>
     <t>pre_ext_method</t>
   </si>
@@ -573,6 +573,12 @@
   </si>
   <si>
     <t>Fossil fuel fires</t>
+  </si>
+  <si>
+    <t>irn</t>
+  </si>
+  <si>
+    <t>Avoid jump in other tranpsort emissions in 2012 (scaling factor extended and is too large for years past 2012)</t>
   </si>
 </sst>
 </file>
@@ -1789,10 +1795,10 @@
   <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C53" sqref="C53"/>
+      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2641,11 +2647,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3482,6 +3488,32 @@
         <v>172</v>
       </c>
     </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>180</v>
+      </c>
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33">
+        <v>1992</v>
+      </c>
+      <c r="G33">
+        <v>2011</v>
+      </c>
+      <c r="H33" t="s">
+        <v>181</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Update to EDGAR v4.3.2 inventory scaling. 1. Include possibility to scale to BC inventory 2. Update mapping files for specific species in order to correct for inventory jumps in certain countries
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/Edgar_scaling_mapping.xlsx
+++ b/input/mappings/scaling/Edgar_scaling_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emcduffie/Documents/GEOS-Chem/CEDS/CEDS_v0611/input/mappings/scaling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A46E3C-CB9B-D84C-82CD-A97A20FF4FE2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6B3FA9-DCF1-D641-B1B0-1F1DFD8665E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13040" yWindow="3420" windowWidth="25360" windowHeight="14640" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2880" yWindow="3360" windowWidth="25360" windowHeight="14640" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
@@ -1795,10 +1795,10 @@
   <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomRight" activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2650,8 +2650,8 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2687,7 +2687,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="B2" t="s">
         <v>137</v>
@@ -2702,15 +2702,18 @@
         <v>9</v>
       </c>
       <c r="F2">
-        <v>1992</v>
+        <v>2000</v>
       </c>
       <c r="G2">
         <v>2012</v>
       </c>
+      <c r="H2" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
         <v>137</v>
@@ -2721,17 +2724,17 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3">
-        <v>2000</v>
-      </c>
-      <c r="G3">
-        <v>2012</v>
+      <c r="E3">
+        <v>1992</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -2748,7 +2751,7 @@
         <v>9</v>
       </c>
       <c r="E4">
-        <v>1992</v>
+        <v>2000</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
@@ -2774,7 +2777,7 @@
         <v>9</v>
       </c>
       <c r="E5">
-        <v>2000</v>
+        <v>2010</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
@@ -2788,7 +2791,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="B6" t="s">
         <v>137</v>
@@ -2800,7 +2803,7 @@
         <v>9</v>
       </c>
       <c r="E6">
-        <v>2010</v>
+        <v>1992</v>
       </c>
       <c r="F6" t="s">
         <v>9</v>
@@ -2814,7 +2817,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="B7" t="s">
         <v>137</v>
@@ -2825,22 +2828,22 @@
       <c r="D7" t="s">
         <v>9</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7">
         <v>1992</v>
       </c>
-      <c r="F7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" t="s">
-        <v>9</v>
+      <c r="G7">
+        <v>2012</v>
       </c>
       <c r="H7" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B8" t="s">
         <v>137</v>
@@ -2866,7 +2869,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B9" t="s">
         <v>137</v>
@@ -2892,7 +2895,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B10" t="s">
         <v>137</v>
@@ -2918,7 +2921,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B11" t="s">
         <v>137</v>
@@ -2944,7 +2947,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B12" t="s">
         <v>137</v>
@@ -2970,7 +2973,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B13" t="s">
         <v>137</v>
@@ -2996,7 +2999,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B14" t="s">
         <v>137</v>
@@ -3022,7 +3025,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B15" t="s">
         <v>137</v>
@@ -3048,7 +3051,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B16" t="s">
         <v>137</v>
@@ -3074,7 +3077,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B17" t="s">
         <v>137</v>
@@ -3100,7 +3103,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B18" t="s">
         <v>137</v>
@@ -3126,7 +3129,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B19" t="s">
         <v>137</v>
@@ -3152,7 +3155,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B20" t="s">
         <v>137</v>
@@ -3178,7 +3181,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B21" t="s">
         <v>137</v>
@@ -3204,7 +3207,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B22" t="s">
         <v>137</v>
@@ -3225,12 +3228,12 @@
         <v>2012</v>
       </c>
       <c r="H22" t="s">
-        <v>147</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B23" t="s">
         <v>137</v>
@@ -3256,7 +3259,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="B24" t="s">
         <v>137</v>
@@ -3282,7 +3285,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="B25" t="s">
         <v>137</v>
@@ -3308,7 +3311,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B26" t="s">
         <v>137</v>
@@ -3334,7 +3337,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B27" t="s">
         <v>137</v>
@@ -3360,7 +3363,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>167</v>
+        <v>141</v>
       </c>
       <c r="B28" t="s">
         <v>137</v>
@@ -3386,7 +3389,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>141</v>
+        <v>168</v>
       </c>
       <c r="B29" t="s">
         <v>137</v>
@@ -3412,10 +3415,10 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>168</v>
-      </c>
-      <c r="B30" t="s">
-        <v>137</v>
+        <v>171</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="C30" t="s">
         <v>9</v>
@@ -3427,21 +3430,21 @@
         <v>9</v>
       </c>
       <c r="F30">
-        <v>1992</v>
+        <v>2000</v>
       </c>
       <c r="G30">
-        <v>2012</v>
-      </c>
-      <c r="H30" t="s">
-        <v>169</v>
+        <v>2008</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>137</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>33</v>
+        <v>180</v>
+      </c>
+      <c r="B31" t="s">
+        <v>35</v>
       </c>
       <c r="C31" t="s">
         <v>9</v>
@@ -3453,21 +3456,21 @@
         <v>9</v>
       </c>
       <c r="F31">
-        <v>2000</v>
+        <v>1992</v>
       </c>
       <c r="G31">
-        <v>2012</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>170</v>
+        <v>2011</v>
+      </c>
+      <c r="H31" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>171</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>33</v>
+        <v>137</v>
+      </c>
+      <c r="B32" t="s">
+        <v>137</v>
       </c>
       <c r="C32" t="s">
         <v>9</v>
@@ -3479,21 +3482,18 @@
         <v>9</v>
       </c>
       <c r="F32">
-        <v>2000</v>
+        <v>1992</v>
       </c>
       <c r="G32">
-        <v>2008</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>172</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>180</v>
-      </c>
-      <c r="B33" t="s">
-        <v>35</v>
+        <v>137</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="C33" t="s">
         <v>9</v>
@@ -3505,13 +3505,13 @@
         <v>9</v>
       </c>
       <c r="F33">
-        <v>1992</v>
+        <v>2000</v>
       </c>
       <c r="G33">
-        <v>2011</v>
-      </c>
-      <c r="H33" t="s">
-        <v>181</v>
+        <v>2012</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>